<commit_message>
debug quantity and price in cart koperasi
</commit_message>
<xml_diff>
--- a/public/uploads/excel/productTypeList.xlsx
+++ b/public/uploads/excel/productTypeList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14DE422-2F01-4005-A3F0-D1DBE576C45F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18F34F0-7CCA-463E-8A21-A5BF7FFAD31B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11064" windowHeight="5112" xr2:uid="{D7C1F6F8-8A5A-41A3-87AF-CE81963DC0EC}"/>
   </bookViews>
@@ -25,24 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>T1 Items</t>
+    <t>name</t>
   </si>
   <si>
-    <t>T2 Items</t>
+    <t>BUKU-BUKU TAMBAHAN T1</t>
   </si>
   <si>
-    <t>T3 Items</t>
-  </si>
-  <si>
-    <t>T4 Items</t>
-  </si>
-  <si>
-    <t>T5 Items</t>
-  </si>
-  <si>
-    <t>name</t>
+    <t>BUKU TULIS/ALAT-ALAT</t>
   </si>
 </sst>
 </file>
@@ -394,40 +385,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99BC05E5-9B50-40DE-95D2-29E7F789EBE0}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>